<commit_message>
Updated code and bug fixes, Release R01.00.10-20141217
</commit_message>
<xml_diff>
--- a/TrackChange.xlsx
+++ b/TrackChange.xlsx
@@ -16,106 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
-  <si>
-    <t>tds.student.sbacossmerge.data</t>
-  </si>
-  <si>
-    <t>GeoComponent</t>
-  </si>
-  <si>
-    <t>new class</t>
-  </si>
-  <si>
-    <t>GeoType</t>
-  </si>
-  <si>
-    <t>LoginInfo</t>
-  </si>
-  <si>
-    <t>new properties added</t>
-  </si>
-  <si>
-    <t>LoginInfoAccomodation</t>
-  </si>
-  <si>
-    <t>for Accomodation class used as inner class in LoginInfo</t>
-  </si>
-  <si>
-    <t>TestResponseReader</t>
-  </si>
-  <si>
-    <t>parse() is changed, as posted xml format changed. parseRequest(), parseResponse() added.</t>
-  </si>
-  <si>
-    <t>TestResponseHandler</t>
-  </si>
-  <si>
-    <t>tds.student.web.handlers</t>
-  </si>
-  <si>
-    <t>TestResponseWriter</t>
-  </si>
-  <si>
-    <t>Lots of changes, response format is changed</t>
-  </si>
-  <si>
-    <t>TestResponseReaderSax</t>
-  </si>
-  <si>
-    <t>Used instead of TestResponseReader.</t>
-  </si>
-  <si>
-    <t>TestShell.axd/updateResponses rest endpoint added. Uses TestResponseReaderSax.</t>
-  </si>
-  <si>
-    <t>MasterShellHandler</t>
-  </si>
-  <si>
-    <t>loginStudent() takes more parameters, LoginInfo of sbacossmerge is used.</t>
-  </si>
-  <si>
-    <t>ContentHandler</t>
-  </si>
-  <si>
-    <t>TestShell.axd/getPageContent rest endpoint added</t>
-  </si>
-  <si>
-    <t>tds.student.web.controls.dummy</t>
-  </si>
-  <si>
-    <t>GlobalJavascript</t>
-  </si>
-  <si>
-    <t>aspx replaced by xhtml</t>
-  </si>
-  <si>
-    <t>tds.student.web.backing</t>
-  </si>
-  <si>
-    <t>LoginBacking</t>
-  </si>
-  <si>
-    <t>processLoginInfo() for parsing 'package' parameter</t>
-  </si>
-  <si>
-    <t>TesteeSax</t>
-  </si>
-  <si>
-    <t>In place of Testee with new properties</t>
-  </si>
-  <si>
-    <t>ItemResponseUpdate</t>
-  </si>
-  <si>
-    <t>with new property '_pageKey'</t>
-  </si>
-  <si>
-    <t>TestShellHandler</t>
-  </si>
-  <si>
-    <t>TestShell.axd/completeTest rest endpoint added</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Scripts</t>
   </si>
@@ -465,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,147 +387,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code and bug fixes, Release R01.00.17-20150121 (corrected)
</commit_message>
<xml_diff>
--- a/TrackChange.xlsx
+++ b/TrackChange.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Scripts</t>
   </si>
@@ -28,6 +28,51 @@
   </si>
   <si>
     <t>changes remaining there to be reverted</t>
+  </si>
+  <si>
+    <t>.mathquill-editable .mq-empty {</t>
+  </si>
+  <si>
+    <t>    min-height: 1em;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>.mathquill-rendered-math .mq-non-leaf, .mathquill-rendered-math .mq-scaled {</t>
+  </si>
+  <si>
+    <t>    vertical-align: middle;</t>
+  </si>
+  <si>
+    <t>custom_eq_editor.css</t>
+  </si>
+  <si>
+    <t>blackbox.js</t>
+  </si>
+  <si>
+    <t>Uncommented line 252-253</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>css/universal/shell.css</t>
+  </si>
+  <si>
+    <t>Line 1437 changed from "margin-top:-25px" to "margin-top:0px"</t>
+  </si>
+  <si>
+    <t>SB-1010</t>
+  </si>
+  <si>
+    <t>SB-622</t>
+  </si>
+  <si>
+    <t>eq item jump</t>
+  </si>
+  <si>
+    <t>print request</t>
   </si>
 </sst>
 </file>
@@ -366,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,9 +422,10 @@
     <col min="1" max="1" width="27.44140625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="73.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,12 +436,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>